<commit_message>
First commit - add service_interactions_api project
</commit_message>
<xml_diff>
--- a/service_interactions.xlsx
+++ b/service_interactions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Jadara\dummy data\fivecustomer\Source Data\newdata lastv2\v1 define drived and deleted columns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Jadara\internship 2025\final Edition\Data Source\service_interactions_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D9D23C5-CF66-4236-B61A-D71F9C96AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07A10A1-BC40-4C6C-B1D1-5A9332CC49A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{9893C6F6-C223-4E50-B7B5-90668964FE53}"/>
   </bookViews>
@@ -6211,9 +6211,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384522AD-F762-42DA-B142-ABBA4C39DEA0}">
   <dimension ref="A1:K1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>